<commit_message>
towards pilot now for realll
</commit_message>
<xml_diff>
--- a/ipa_1_2/myUtils/instructions.xlsx
+++ b/ipa_1_2/myUtils/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_1_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD5B477-998D-4AB0-A004-8FE28DD6AEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE77AB20-63E2-4340-A0DF-E338BE87A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="120">
   <si>
     <t>phase</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>During Profile Presentation</t>
-  </si>
-  <si>
-    <t>הסוף</t>
   </si>
   <si>
     <t>text_he</t>
@@ -132,9 +129,6 @@
     <t>will</t>
   </si>
   <si>
-    <t>קראתי את עמוד זה</t>
-  </si>
-  <si>
     <t>אני בן 18 או יותר</t>
   </si>
   <si>
@@ -150,14 +144,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם, הדומה לך ביותר מבחינת כל התכונות והמאפיינים. 
-קח זמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום כאן את ראשי התיבות של שמו.ה</t>
-  </si>
-  <si>
-    <t>מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם, הדומה לך ביותר מבחינת כל התכונות והמאפיינים. 
-קח זמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום את ראשי התיבות של שמו.ה</t>
-  </si>
-  <si>
     <t>lowSimilarity</t>
   </si>
   <si>
@@ -183,10 +169,6 @@
   </si>
   <si>
     <t>End Screen</t>
-  </si>
-  <si>
-    <t>מבין כל האנשים שאת יכול לחשוב עליהם, בחרי את האדם, הדומה לך ביותר מבחינת כל התכונות והמאפיינים. 
-קחי זמן וחשבי היטב, רק לאחר שאת בטוחה בבחירתך, רשמי כאן את ראשי התיבות של שמו.ה</t>
   </si>
   <si>
     <t>---</t>
@@ -243,12 +225,6 @@
   </si>
   <si>
     <t>concent_agreement</t>
-  </si>
-  <si>
-    <t>מאשר את כלל הפרטים הנ''ל ומסכים מרצוני החופשי להשתתף במחקר זה</t>
-  </si>
-  <si>
-    <t>מאשרת את כלל הפרטים הנ''ל ומסכימה מרצוני החופשי להשתתף במחקר זה</t>
   </si>
   <si>
     <t>המחשב בדק את תשובותיך ומצא כי מספר טעויות. נבקש ממך לבצע מטלה קצרה זו שוב על מנת שתוכל להמשיך בניסוי. 
@@ -303,26 +279,6 @@
 במידת הצורך פני לנסיינ.ית לעזרה.</t>
   </si>
   <si>
-    <t>חשבי על {}, האדם שציינת כהכי פחות דומה לך. חשבי עד כמה את מרגישה שאת ו-{} דומים.
-אנא תדרגי את מידת הדמיון בינך לבין {}. השתמשי בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.  
-ככל שמידת החפיפה גדולה יותר, כך זה אומר שאת מרגישה שאת ו-{} דומים יותר.</t>
-  </si>
-  <si>
-    <t>חשוב על {}, האדם שציינת כהכי פחות דומה לך. חשוב עד כמה אתה מרגיש שאתה ו-{} דומים.
-אנא תדרג את מידת הדמיון בינך לבין {}. השתמש בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.
-ככל שמידת החפיפה גדולה יותר, כך זה אומר שאתה מרגיש שאתה ו-{} דומים יותר.</t>
-  </si>
-  <si>
-    <t>חשבי על {}, האדם שציינת כדומה לך ביותר. חשבי עד כמה את מרגישה שאת ו-{} דומים.
-אנא תדרגי את מידת הדמיון בינך לבין {}. השתמשי בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.  
-ככל שמידת החפיפה גדולה יותר, כך זה אומר שאת מרגישה שאת ו-{} דומים יותר.</t>
-  </si>
-  <si>
-    <t>חשוב על {}, האדם שציינת כדומה לך ביותר. חשוב עד כמה אתה מרגיש שאתה ו-{},  דומים.
-אנא תדרג את מידת הדמיון בינך לבין {}. השתמש בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.
-ככל שמידת החפיפה גדולה יותר, כך זה אומר שאתה מרגיש שאתה ו-{} דומים יותר.</t>
-  </si>
-  <si>
     <t>אצל רובנו התפיסה של מי שאנחנו מחולקת לאיך שאנחנו תופסים את עצמנו כעת ואיך שאנחנו היינו רוצים להיות, כלומר איזה אדם היינו רוצים להיות במצב אידאלי.
 בחלק זה של הניסוי זה תתבקש לענות פעם נוספת על אותן שאלות כמו בהתחלה 
 אשר עוסקות במאפיינים השונים שלך, אלא שהפעם תתבקש לדרג את המאפיינים לפי איך שהיית רוצה להיות ולא לפי איך שאתה בפועל. 
@@ -348,24 +304,6 @@
     <t>כעת את מתבקשת לדווח על מידת הדמיון שאת חווה בינך לבין האדם האחר. השתמשי בכפתורים על מנת לשנות את מידת החפיפה. ככל שמידת החפיפה גדולה יותר - כך הדבר משקף חוויית דמיון גבוהה יותר.</t>
   </si>
   <si>
-    <t>האימון הסתיים וכעת תמשיכי בביצוע מטלה זו. המטלה זהה מאוד לאימון מלבד מספר הבדלים. בשונה מבאימון, בשלב זה לא יוצגו שני מעגלי החפיפה הנוספים (בינך לבין האדם שציינת כדומה לך ביותר, ובינך לבין האדם שציינת כשונה ממך ביותר), כמו כן צבע מעגלי הדיווח יהיה כעת אפור.
-&lt;br&gt;המטלה נותרת זהה - יש להתבונן במאפיינים שמוצגים, ניתן להתבונן שוב במידת הצורך, כאשר מטרתך תוך כדי ההתבוננות במאפיינים היא לנסות להכיר את אותו אדם. לאחר מכן יש לדווח על תחושת הדמיון בינך לבין האדם שצפית בתכונותיו, בהתאם לחוויתך האישית והפנימית.
-&lt;br&gt;&lt;br&gt;אם יש לך שאלות, ניתן לפנות כעת לנסיינ.ית</t>
-  </si>
-  <si>
-    <t>האימון הסתיים וכעת תמשיך בביצוע מטלה זו. המטלה זהה מאוד לאימון מלבד מספר הבדלים. בשונה מבאימון, בשלב זה לא יוצגו שני מעגלי החפיפה הנוספים (בינך לבין האדם שציינת כדומה לך ביותר, ובינך לבין האדם שציינת כשונה ממך ביותר), כמו כן צבע מעגלי הדיווח יהיה כעת אפור.
-&lt;br&gt;המטלה נותרת זהה - יש להתבונן במאפיינים שמוצגים, ניתן להתבונן שוב במידת הצורך, כאשר מטרתך תוך כדי ההתבוננות במאפיינים היא לנסות להכיר את אותו אדם. לאחר מכן יש לדווח על תחושת הדמיון בינך לבין האדם שצפית בתכונותיו, בהתאם לחוויתך האישית והפנימית.
-&lt;br&gt;&lt;br&gt;אם יש לך שאלות, ניתן לפנות כעת לנסיינ.ית</t>
-  </si>
-  <si>
-    <t>כעת, מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם הכי פחות דומה לך מבחינת כל התכונות והמאפיינים. 
-קח זמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום כאן את ראשי התיבות של שמו.ה</t>
-  </si>
-  <si>
-    <t>כעת, מבין כל האנשים שאת יכול לחשוב עליהם, בחרי את האדם הכי פחות דומה לך מבחינת כל התכונות והמאפיינים. 
-קחי זמן וחשבי היטב, רק לאחר שאת בטוחה בבחירתך, רשמי כאן את ראשי התיבות של שמו.ה</t>
-  </si>
-  <si>
     <t>כעת תתבקשי לענות על אותן השאלות, אלו שקודם ענית עבור עצמך, אך הפעם עבור {}, האדם שציינת &lt;strong&gt; כדומה לך ביותר&lt;/strong&gt;. כמובן, שאינך יכולה לדעת את התשובות במדויק, לכן נסי לחשוב מה תהיה השתובה של {}, לדעתך. 
 &lt;br&gt;יש ללחוץ על הסמן על מנת לבחור את המיקום על הסקאלה. לאחר בחירת מיקום הסמן, לחצי על הכפתור אשר יופיע בתחתית המסך.</t>
   </si>
@@ -459,6 +397,111 @@
   </si>
   <si>
     <t>PrePresntationInstructions.JPG</t>
+  </si>
+  <si>
+    <t>קראתי עמוד זה</t>
+  </si>
+  <si>
+    <t>אני מאשר ומסכים להשתתף במחקר זה מרצוני החופשי</t>
+  </si>
+  <si>
+    <t>אני מאשרת ומסכימה להשתתף במחקר זה מרצוני החופשי</t>
+  </si>
+  <si>
+    <t>GeneralPhase</t>
+  </si>
+  <si>
+    <t>הבא</t>
+  </si>
+  <si>
+    <t>nextButtonText</t>
+  </si>
+  <si>
+    <t>מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם, הדומה לך ביותר מבחינת כל התכונות והמאפיינים. 
+קח את הזמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום את ראשי התיבות של שמו.ה</t>
+  </si>
+  <si>
+    <t>כעת, מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם הכי פחות דומה לך מבחינת כל התכונות והמאפיינים. 
+קח את הזמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום כאן את ראשי התיבות של שמו.ה</t>
+  </si>
+  <si>
+    <t>חשוֹב על {}, האדם שציינת כדומה לך ביותר. חשוב עד כמה אתה מרגיש שאתה ו-{},  דומים.
+אנא תדרג את מידת הדמיון בינך לבין {}. השתמש בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.
+ככל שמידת החפיפה גדולה יותר, כך מידת הדמיון בינכם גדולה יותר.</t>
+  </si>
+  <si>
+    <t>חשוֹב על {}, האדם שציינת כהכי פחות דומה לך. חשוב עד כמה אתה מרגיש שאתה ו-{} דומים.
+אנא תדרג את מידת הדמיון בינך לבין {}. השתמש בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.
+ככל שמידת החפיפה גדולה יותר, כך מידת הדמיון בינכם גדולה יותר.</t>
+  </si>
+  <si>
+    <t>כעת, מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם הכי פחות דומה לך מבחינת כל התכונות והמאפיינים. 
+קח את הזמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום כאן את ראשי התיבות של שמו או של שמה</t>
+  </si>
+  <si>
+    <t>כעת, מבין כל האנשים שאת יכול לחשוב עליהם, בחרי את האדם הכי פחות דומה לך מבחינת כל התכונות והמאפיינים. 
+קחי את הזמן וחשבי היטב, רק לאחר שאת בטוחה בבחירתך, רשמי כאן את ראשי התיבות של שמו או של שמה</t>
+  </si>
+  <si>
+    <t>מבין כל האנשים שאת יכול לחשוב עליהם, בחרי את האדם, הדומה לך ביותר מבחינת כל התכונות והמאפיינים. 
+קחי את הזמן וחשבי היטב, רק לאחר שאת בטוחה בבחירתך, רשמי כאן את ראשי התיבות של שמו או של שמה</t>
+  </si>
+  <si>
+    <t>מבין כל האנשים שאתה יכול לחשוב עליהם, בחר את האדם, הדומה לך ביותר מבחינת כל התכונות והמאפיינים. 
+קח את הזמן וחשוב היטב, רק לאחר שאתה בטוח בבחירתך, רשום את ראשי התיבות של שמו או של שמה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חשוֹב על {}, האדם שציינת כדומה לך ביותר. חשוב עד כמה אתה מרגיש שאתה ו-{} דומים.
+אנא דרג את מידת הדמיון בינך לבין {}. השתמש בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.
+ככל שמידת החפיפה גדולה יותר, כך מידת הדמיון בינכם גדולה יותר. השתמש בשני הכפתורים עד שתגיע לחפיפה המדויקת ביותר לדעתך. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">חִשבי על {}, האדם שציינת כדומה לך ביותר. חשבי עד כמה את מרגישה שאת ו-{} דומים.
+אנא דרגי את מידת הדמיון בינך לבין {}. השתמשי בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.  
+ככל שמידת החפיפה גדולה יותר, כך מידת הדמיון בינכם גדולה יותר. השתמשי בשני הכפתורים עד שתגיעי לחפיפה המדויקת ביותר לדעתך. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">חשוֹב על {}, האדם שציינת כהכי פחות דומה לך. חשוב עד כמה אתה מרגיש שאתה ו-{} דומים.
+אנא דרג את מידת הדמיון בינך לבין {}. השתמש בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.
+ככל שמידת החפיפה גדולה יותר, כך מידת הדמיון בינכם גדולה יותר. השתמש בשני הכפתורים עד שתגיע לחפיפה המדויקת ביותר לדעתך. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">חִשבי על {}, האדם שציינת כהכי פחות דומה לך. חשבי עד כמה את מרגישה שאת ו-{} דומים.
+אנא דרגי את מידת הדמיון בינך לבין {}. השתמשי בכפתורים "יותר" או "פחות" על מנת להגדיל או להקטין את מידת החפיפה בין העיגולים.  
+ככל שמידת החפיפה גדולה יותר, כך מידת הדמיון בינכם גדולה יותר. השתמשי בשני הכפתורים עד שתגיעי לחפיפה המדויקת ביותר לדעתך. </t>
+  </si>
+  <si>
+    <t>האימון הסתיים וכעת תמשיך בביצוע מטלה זו. המטלה זהה מאוד לאימון מלבד מספר הבדלים. בשונה מבאימון, בשלב זה לא יוצגו שני מעגלי החפיפה הנוספים (בינך לבין האדם שציינת כדומה לך ביותר, ובינך לבין האדם שציינת כשונה ממך ביותר).
+&lt;br&gt;המטלה נותרת זהה - יש להתבונן במאפיינים שמוצגים, ניתן להתבונן שוב במידת הצורך, כאשר מטרתך תוך כדי ההתבוננות במאפיינים היא לנסות להכיר את אותו אדם. לאחר מכן יש לדווח על תחושת הדמיון בינך לבין האדם שצפית בתכונותיו, בהתאם לחוויתך האישית והפנימית.
+&lt;br&gt;&lt;br&gt;אם יש לך שאלות, ניתן לפנות כעת לנסיינ.ית</t>
+  </si>
+  <si>
+    <t>האימון הסתיים וכעת תמשיכי בביצוע מטלה זו. המטלה זהה מאוד לאימון מלבד מספר הבדלים. בשונה מבאימון, בשלב זה לא יוצגו שני מעגלי החפיפה הנוספים (בינך לבין האדם שציינת כדומה לך ביותר, ובינך לבין האדם שציינת כשונה ממך ביותר).
+&lt;br&gt;המטלה נותרת זהה - יש להתבונן במאפיינים שמוצגים, ניתן להתבונן שוב במידת הצורך, כאשר מטרתך תוך כדי ההתבוננות במאפיינים היא לנסות להכיר את אותו אדם. לאחר מכן יש לדווח על תחושת הדמיון בינך לבין האדם שצפית בתכונותיו, בהתאם לחוויתך האישית והפנימית.
+&lt;br&gt;&lt;br&gt;אם יש לך שאלות, ניתן לפנות כעת לנסיינ.ית</t>
+  </si>
+  <si>
+    <t>endTitle</t>
+  </si>
+  <si>
+    <t>הניסוי הסתיים!</t>
+  </si>
+  <si>
+    <t>endSubTitle</t>
+  </si>
+  <si>
+    <t>תודה על השתתפותך : )</t>
+  </si>
+  <si>
+    <t>endInstructions</t>
+  </si>
+  <si>
+    <t>הנתונים נשמרו, קראי כעת לנסיין.ית על מנת שהיא או הוא יוכלו ליסגור את הניסוי. 
+בעוד מספר דקות תקבלי תשלום או קרדיט ובנוסף יחושב עבורך הבונוס כתלות בביצועיך.</t>
+  </si>
+  <si>
+    <t>הנתונים נשמרו, קרא כעת לנסיין.ית על מנת שהיא או הוא יוכלו ליסגור את הניסוי.
+בעוד מספר דקות תקבל תשלום או קרדיט ובנוסף יחושב עבורך הבונוס כתלות בביצועיך.</t>
   </si>
 </sst>
 </file>
@@ -502,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,6 +571,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,864 +861,924 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>87</v>
+        <v>109</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>96</v>
+        <v>73</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>45</v>
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>37</v>
+      <c r="C17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>90</v>
+        <v>15</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>100</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>107</v>
+        <v>8</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>37</v>
+        <v>8</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ready to sudents pilot
</commit_message>
<xml_diff>
--- a/ipa_1_2/myUtils/instructions.xlsx
+++ b/ipa_1_2/myUtils/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_1_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F393660A-01D0-44AB-AD65-8A5177E77CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D15D64-C656-482D-B90D-4104D489767E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes for friends pilot
</commit_message>
<xml_diff>
--- a/ipa_1_2/myUtils/instructions.xlsx
+++ b/ipa_1_2/myUtils/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_1_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A87107-226E-4F45-8C0B-002D9F4FA6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B2E594-3353-4176-AC0F-35CB35747579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
   <si>
     <t>phase</t>
   </si>
@@ -449,14 +449,6 @@
 &lt;br&gt;חשוב מאוד שהערכת הדמיון שלך תהיה מבוססת על חווייתך האישית האמיתית.</t>
   </si>
   <si>
-    <t>אנא דווחי על מידת הדמיון שאת חווה בינך לבין האדם האחר.
-&lt;br&gt;השתמש בכפתורים על מנת לשנות את מידת החפיפה. ככל שמידת החפיפה גדולה יותר - כך הדבר משקף חוויית דמיון גבוהה יותר.</t>
-  </si>
-  <si>
-    <t>אנא דווח על מידת הדמיון שאתה חווה בינך לבין האדם האחר.
-&lt;br&gt;השתמש בכפתורים על מנת לשנות את מידת החפיפה. ככל שמידת החפיפה גדולה יותר - כך הדבר משקף חוויית דמיון גבוהה יותר.</t>
-  </si>
-  <si>
     <t>מיוד יוצג פרופיל של משתתף חדש. התבונן היטב בהעדפות והמאפיינים השונים ונסה להכיר את אותו אדם.</t>
   </si>
   <si>
@@ -499,6 +491,17 @@
   <si>
     <t xml:space="preserve">בשלב הבא יוצגו שני מעגלים, אלו מעגלי דיווח חווית הדמיון. עליך להשתמש בשני הכפתורים "+" -" על מנת להגדיל או להקטין את מידת החפיפה ביניהם ובכך לדווח עד כמה אתה מרגיש שאתה והאדם המתואר דומים. חפיפה מוחלטת משמעה דמיון גבוה ביותר והיעדר חפיפה משמעו דמיון נמוך ביותר. המצב ההתחלתי של המעגלים יהיה בהיעדר מוחלט של חפיפה.
 </t>
+  </si>
+  <si>
+    <t>כעת יוצג בשנית הפרופיל של אותו משתתף, זה שצפית בו כעת. 
+&lt;br&gt;
+כעת תוכל לעבור מהר יותר בין במאפיינים או ההעדפות ולהתעקב היכן שתרצה. מטרתך נותרת לנסות להכיר את אותו אדם ובסופו של דבר להעריך עד כמה אתה מרגיש שאתם דומים.</t>
+  </si>
+  <si>
+    <t>אנא דווח על מידת הדמיון שאתה חווה בינך לבין האדם האחר. השתמש בכפתורים על מנת לשנות את מידת החפיפה. ככל שמידת החפיפה גדולה יותר - כך הדבר משקף חוויית דמיון גבוהה יותר.</t>
+  </si>
+  <si>
+    <t>אנא דווחי על מידת הדמיון שאת חווה בינך לבין האדם האחר. השתמש בכפתורים על מנת לשנות את מידת החפיפה. ככל שמידת החפיפה גדולה יותר - כך הדבר משקף חוויית דמיון גבוהה יותר.</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,13 +1531,13 @@
         <v>8</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1633,13 +1636,13 @@
         <v>8</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1695,13 +1698,13 @@
         <v>8</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -1779,13 +1782,13 @@
         <v>51</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1800,20 +1803,20 @@
         <v>61</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>5</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>63</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>64</v>
@@ -1842,13 +1845,13 @@
         <v>8</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>

</xml_diff>